<commit_message>
final updates to composite
</commit_message>
<xml_diff>
--- a/UGDG/Behavioral_Analysis/covariates/Composite_Reward.xlsx
+++ b/UGDG/Behavioral_Analysis/covariates/Composite_Reward.xlsx
@@ -13,7 +13,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Composite_Reward</t>
+  </si>
+  <si>
+    <t>Composite_Reward_Squared</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Composite_Reward</t>
+  </si>
+  <si>
+    <t>Composite_Reward_Squared</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Composite_Reward</t>
+  </si>
+  <si>
+    <t>Composite_Reward_Squared</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Composite_Reward</t>
+  </si>
+  <si>
+    <t>Composite_Reward_Squared</t>
+  </si>
   <si>
     <t>Subject</t>
   </si>
@@ -159,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -181,11 +217,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -201,6 +241,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -220,13 +264,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">

</xml_diff>